<commit_message>
full table with weather
</commit_message>
<xml_diff>
--- a/stadiums_nfl.xlsx
+++ b/stadiums_nfl.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xiaoqi\Desktop\Data Analytics Course\Homework\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xiaoqi\Desktop\Data Analytics Course\Homework\Final Project\New Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BAF0D6-6807-4421-BB3E-33F1280C1342}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177D9D43-85A7-4901-9017-5C94E1A0FE8C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="444">
   <si>
     <t>Geo Point</t>
   </si>
@@ -325,9 +325,6 @@
     <t>North</t>
   </si>
   <si>
-    <t>Chicago Bers</t>
-  </si>
-  <si>
     <t>42.0918799131, -71.2649100654</t>
   </si>
   <si>
@@ -667,9 +664,6 @@
     <t>Shares stadium with Giants(NFL) and Jets(NFL)</t>
   </si>
   <si>
-    <t>New York Giants/ NewYork Jets</t>
-  </si>
-  <si>
     <t>25.9580100153, -80.2388899544</t>
   </si>
   <si>
@@ -805,9 +799,6 @@
     <t>-90.18854000000</t>
   </si>
   <si>
-    <t>St. Louis Rams</t>
-  </si>
-  <si>
     <t>39.2779000046, -76.6227000055</t>
   </si>
   <si>
@@ -1250,6 +1241,117 @@
   </si>
   <si>
     <t>07073</t>
+  </si>
+  <si>
+    <t>Chicago Bears</t>
+  </si>
+  <si>
+    <t>New York Giants</t>
+  </si>
+  <si>
+    <t>New York Jets</t>
+  </si>
+  <si>
+    <t>Saint Louis Rams</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>JAX</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>BUF</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>CIN</t>
+  </si>
+  <si>
+    <t>NYG</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>ARI</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>OAK</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>TEN</t>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>NYJ</t>
+  </si>
+  <si>
+    <t>Team Abbreviation</t>
   </si>
 </sst>
 </file>
@@ -2100,10 +2202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG32"/>
+  <dimension ref="A1:AH33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M2" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2111,9 +2213,10 @@
     <col min="7" max="8" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2213,8 +2316,11 @@
       <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" s="1" t="s">
+        <v>443</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
@@ -2293,8 +2399,11 @@
       <c r="AG2" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="AH2" t="s">
+        <v>411</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
@@ -2373,8 +2482,11 @@
       <c r="AG3" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="AH3" t="s">
+        <v>412</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
@@ -2450,8 +2562,11 @@
       <c r="AG4" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="AH4" t="s">
+        <v>413</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
@@ -2530,8 +2645,11 @@
       <c r="AG5" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="AH5" t="s">
+        <v>414</v>
+      </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>90</v>
       </c>
@@ -2605,15 +2723,18 @@
         <v>51</v>
       </c>
       <c r="AG6" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>35</v>
@@ -2634,37 +2755,37 @@
         <v>40220</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="T7" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="S7" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="T7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="W7" s="2">
         <v>1</v>
       </c>
       <c r="X7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y7" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="Z7" s="2" t="s">
         <v>46</v>
@@ -2673,7 +2794,7 @@
         <v>47</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AC7" s="2" t="s">
         <v>63</v>
@@ -2688,15 +2809,18 @@
         <v>51</v>
       </c>
       <c r="AG7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>35</v>
@@ -2717,34 +2841,34 @@
         <v>40220</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="U8" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="W8" s="2">
         <v>2</v>
       </c>
       <c r="X8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y8" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="Z8" s="2" t="s">
         <v>46</v>
@@ -2765,15 +2889,18 @@
         <v>51</v>
       </c>
       <c r="AG8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>35</v>
@@ -2794,37 +2921,37 @@
         <v>40220</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>83</v>
       </c>
       <c r="S9" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="U9" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="W9" s="2">
         <v>4</v>
       </c>
       <c r="X9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y9" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="Z9" s="2" t="s">
         <v>46</v>
@@ -2833,7 +2960,7 @@
         <v>47</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AC9" s="2" t="s">
         <v>49</v>
@@ -2848,15 +2975,18 @@
         <v>51</v>
       </c>
       <c r="AG9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>35</v>
@@ -2877,34 +3007,34 @@
         <v>40220</v>
       </c>
       <c r="J10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="R10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="U10" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="V10" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="W10" s="2">
         <v>10</v>
       </c>
       <c r="X10" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y10" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="Z10" s="2" t="s">
         <v>46</v>
@@ -2913,7 +3043,7 @@
         <v>47</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AC10" s="2" t="s">
         <v>49</v>
@@ -2928,15 +3058,18 @@
         <v>51</v>
       </c>
       <c r="AG10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>35</v>
@@ -2957,34 +3090,34 @@
         <v>40220</v>
       </c>
       <c r="J11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="R11" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="S11" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="U11" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="V11" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="W11" s="2">
         <v>5</v>
       </c>
       <c r="X11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y11" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="Z11" s="2" t="s">
         <v>46</v>
@@ -3005,15 +3138,18 @@
         <v>51</v>
       </c>
       <c r="AG11" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>35</v>
@@ -3034,37 +3170,37 @@
         <v>40220</v>
       </c>
       <c r="J12" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="R12" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="S12" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="U12" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="V12" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="W12" s="2">
         <v>5</v>
       </c>
       <c r="X12" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y12" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="Y12" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="Z12" s="2" t="s">
         <v>46</v>
@@ -3073,7 +3209,7 @@
         <v>47</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AC12" s="2" t="s">
         <v>49</v>
@@ -3085,18 +3221,21 @@
         <v>64035</v>
       </c>
       <c r="AF12" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG12" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="AG12" s="2" t="s">
+      <c r="AH12" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>35</v>
@@ -3117,37 +3256,37 @@
         <v>40220</v>
       </c>
       <c r="J13" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="R13" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="S13" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="U13" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="U13" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="V13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="W13" s="2">
         <v>4</v>
       </c>
       <c r="X13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y13" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="Z13" s="2" t="s">
         <v>46</v>
@@ -3156,7 +3295,7 @@
         <v>47</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AC13" s="2" t="s">
         <v>49</v>
@@ -3168,18 +3307,21 @@
         <v>71228</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>35</v>
@@ -3200,34 +3342,34 @@
         <v>40220</v>
       </c>
       <c r="J14" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="Q14" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="R14" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="R14" s="2" t="s">
+      <c r="S14" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="U14" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="U14" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="V14" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="W14" s="2">
         <v>5</v>
       </c>
       <c r="X14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y14" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="Z14" s="2" t="s">
         <v>46</v>
@@ -3248,15 +3390,18 @@
         <v>51</v>
       </c>
       <c r="AG14" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>35</v>
@@ -3274,34 +3419,34 @@
         <v>40220</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="R15" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="S15" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="U15" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="S15" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="U15" s="2" t="s">
+      <c r="V15" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="W15" s="2">
         <v>2</v>
       </c>
       <c r="X15" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y15" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="Y15" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="Z15" s="2" t="s">
         <v>46</v>
@@ -3310,7 +3455,7 @@
         <v>47</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AC15" s="2" t="s">
         <v>49</v>
@@ -3325,15 +3470,18 @@
         <v>51</v>
       </c>
       <c r="AG15" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>35</v>
@@ -3354,34 +3502,34 @@
         <v>40220</v>
       </c>
       <c r="J16" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>83</v>
       </c>
       <c r="S16" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="V16" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="W16" s="2">
         <v>4</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="Z16" s="2" t="s">
         <v>46</v>
@@ -3390,7 +3538,7 @@
         <v>47</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AC16" s="2" t="s">
         <v>63</v>
@@ -3405,15 +3553,18 @@
         <v>51</v>
       </c>
       <c r="AG16" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>35</v>
@@ -3431,34 +3582,34 @@
         <v>40220</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q17" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="R17" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="S17" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="R17" s="2" t="s">
+      <c r="U17" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="S17" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="V17" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="W17" s="2">
         <v>5</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="Z17" s="2" t="s">
         <v>46</v>
@@ -3476,18 +3627,21 @@
         <v>63000</v>
       </c>
       <c r="AF17" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AG17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>35</v>
@@ -3508,34 +3662,34 @@
         <v>40220</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="R18" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="S18" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="U18" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="S18" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="V18" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="W18" s="2">
         <v>6</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Z18" s="2" t="s">
         <v>46</v>
@@ -3553,18 +3707,21 @@
         <v>71500</v>
       </c>
       <c r="AF18" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AG18" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>35</v>
@@ -3585,34 +3742,34 @@
         <v>40220</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q19" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="R19" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="S19" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="U19" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="S19" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="V19" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="W19" s="2">
         <v>7</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Z19" s="2" t="s">
         <v>46</v>
@@ -3630,18 +3787,21 @@
         <v>66965</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AG19" s="2" t="s">
-        <v>261</v>
+        <v>177</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>410</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>428</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>35</v>
@@ -3662,34 +3822,34 @@
         <v>40220</v>
       </c>
       <c r="J20" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="R20" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="S20" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="U20" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="R20" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>269</v>
-      </c>
       <c r="V20" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="W20" s="2">
         <v>3</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="Z20" s="2" t="s">
         <v>46</v>
@@ -3710,15 +3870,18 @@
         <v>51</v>
       </c>
       <c r="AG20" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>429</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>35</v>
@@ -3739,37 +3902,37 @@
         <v>40220</v>
       </c>
       <c r="J21" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="S21" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="T21" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="U21" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="S21" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="V21" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="W21" s="2">
         <v>5</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="Z21" s="2" t="s">
         <v>46</v>
@@ -3787,18 +3950,21 @@
         <v>64111</v>
       </c>
       <c r="AF21" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG21" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>430</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>35</v>
@@ -3819,34 +3985,34 @@
         <v>40220</v>
       </c>
       <c r="J22" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="R22" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="S22" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="U22" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="R22" s="2" t="s">
+      <c r="V22" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="S22" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="V22" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="W22" s="2">
         <v>9</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="Z22" s="2" t="s">
         <v>46</v>
@@ -3864,18 +4030,21 @@
         <v>63400</v>
       </c>
       <c r="AF22" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AG22" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>431</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>35</v>
@@ -3896,34 +4065,34 @@
         <v>40220</v>
       </c>
       <c r="J23" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="S23" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="U23" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="V23" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="S23" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="V23" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="W23" s="2">
         <v>5</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="Z23" s="2" t="s">
         <v>46</v>
@@ -3944,15 +4113,18 @@
         <v>51</v>
       </c>
       <c r="AG23" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>432</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>35</v>
@@ -3973,34 +4145,34 @@
         <v>40220</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="R24" s="2" t="s">
         <v>58</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="W24" s="2">
         <v>9</v>
       </c>
       <c r="X24" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="Z24" s="2" t="s">
         <v>46</v>
@@ -4009,7 +4181,7 @@
         <v>47</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>63</v>
@@ -4024,15 +4196,18 @@
         <v>51</v>
       </c>
       <c r="AG24" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>433</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>35</v>
@@ -4053,34 +4228,34 @@
         <v>40220</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="R25" s="2" t="s">
         <v>58</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="W25" s="2">
         <v>9</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Z25" s="2" t="s">
         <v>46</v>
@@ -4101,15 +4276,18 @@
         <v>51</v>
       </c>
       <c r="AG25" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>434</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>35</v>
@@ -4130,34 +4308,34 @@
         <v>40220</v>
       </c>
       <c r="J26" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="R26" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="S26" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="Q26" s="2" t="s">
+      <c r="U26" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="R26" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="S26" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>336</v>
-      </c>
       <c r="V26" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="W26" s="2">
         <v>4</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="Z26" s="2" t="s">
         <v>46</v>
@@ -4166,7 +4344,7 @@
         <v>47</v>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="AC26" s="2" t="s">
         <v>63</v>
@@ -4181,15 +4359,18 @@
         <v>51</v>
       </c>
       <c r="AG26" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>435</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>35</v>
@@ -4210,34 +4391,34 @@
         <v>40220</v>
       </c>
       <c r="J27" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="S27" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="U27" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="Q27" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="S27" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="U27" s="2" t="s">
-        <v>347</v>
-      </c>
       <c r="V27" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="W27" s="2">
         <v>7</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="Z27" s="2" t="s">
         <v>46</v>
@@ -4258,15 +4439,18 @@
         <v>51</v>
       </c>
       <c r="AG27" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>436</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>35</v>
@@ -4287,34 +4471,34 @@
         <v>40220</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="R28" s="2" t="s">
         <v>42</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="W28" s="2">
         <v>3</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Y28" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="Z28" s="2" t="s">
         <v>46</v>
@@ -4323,7 +4507,7 @@
         <v>47</v>
       </c>
       <c r="AB28" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="AC28" s="2" t="s">
         <v>63</v>
@@ -4338,15 +4522,18 @@
         <v>51</v>
       </c>
       <c r="AG28" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>437</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>35</v>
@@ -4367,34 +4554,34 @@
         <v>40220</v>
       </c>
       <c r="J29" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="S29" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="U29" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="Q29" s="2" t="s">
+      <c r="V29" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="S29" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="U29" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="V29" s="2" t="s">
-        <v>369</v>
       </c>
       <c r="W29" s="2">
         <v>3</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="Z29" s="2" t="s">
         <v>46</v>
@@ -4415,15 +4602,18 @@
         <v>51</v>
       </c>
       <c r="AG29" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>438</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>35</v>
@@ -4444,34 +4634,34 @@
         <v>40220</v>
       </c>
       <c r="J30" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="R30" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="S30" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="Q30" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="R30" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="S30" s="4" t="s">
-        <v>379</v>
-      </c>
       <c r="U30" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="W30" s="2">
         <v>8</v>
       </c>
       <c r="X30" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="Y30" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="Z30" s="2" t="s">
         <v>46</v>
@@ -4480,7 +4670,7 @@
         <v>47</v>
       </c>
       <c r="AB30" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="AC30" s="2" t="s">
         <v>63</v>
@@ -4495,15 +4685,18 @@
         <v>51</v>
       </c>
       <c r="AG30" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>439</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>35</v>
@@ -4524,37 +4717,37 @@
         <v>40220</v>
       </c>
       <c r="J31" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="R31" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="S31" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="T31" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="U31" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="S31" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="T31" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="U31" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="V31" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="W31" s="2">
         <v>6</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="Y31" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="Z31" s="2" t="s">
         <v>46</v>
@@ -4563,7 +4756,7 @@
         <v>47</v>
       </c>
       <c r="AB31" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="AC31" s="2" t="s">
         <v>49</v>
@@ -4575,18 +4768,21 @@
         <v>72968</v>
       </c>
       <c r="AF31" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG31" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>440</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>35</v>
@@ -4604,34 +4800,34 @@
         <v>40220</v>
       </c>
       <c r="J32" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="S32" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="U32" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="Q32" s="2" t="s">
+      <c r="V32" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="S32" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="U32" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="V32" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="W32" s="2">
         <v>6</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="Y32" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="Z32" s="2" t="s">
         <v>46</v>
@@ -4649,10 +4845,93 @@
         <v>80000</v>
       </c>
       <c r="AF32" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AG32" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="3">
+        <v>40220</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="W33" s="2">
+        <v>2</v>
+      </c>
+      <c r="X33" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y33" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="Z33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB33" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE33" s="2">
+        <v>82500</v>
+      </c>
+      <c r="AF33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG33" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>